<commit_message>
runRL for until one node dies and results stuff
</commit_message>
<xml_diff>
--- a/pyFiles/RL/Results/New Results/ResultsDQNdecayEpsilon.xlsx
+++ b/pyFiles/RL/Results/New Results/ResultsDQNdecayEpsilon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozho1\Desktop\Thesis Code\ThesisWorkCybercom\pyFiles\RL\Results\New Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91939105-44C3-4D0C-B8B0-D284F0BB5B90}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A1ED5E-573A-4143-9FD5-1242C697545A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="18">
   <si>
     <t>Controller</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Until all node dies</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -531,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2693EA75-5C63-4FDE-887F-C7326CFE699C}">
-  <dimension ref="A1:R99"/>
+  <dimension ref="A1:R109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="E50" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +649,15 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
+      <c r="B6">
+        <v>236127</v>
+      </c>
+      <c r="C6">
+        <v>1227</v>
+      </c>
+      <c r="D6">
+        <v>48.552244900001099</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
@@ -666,6 +678,15 @@
       <c r="A7" s="1">
         <v>2</v>
       </c>
+      <c r="B7">
+        <v>122988</v>
+      </c>
+      <c r="C7">
+        <v>639</v>
+      </c>
+      <c r="D7">
+        <v>43.580299800000397</v>
+      </c>
       <c r="G7">
         <v>1</v>
       </c>
@@ -686,6 +707,15 @@
       <c r="A8" s="1">
         <v>3</v>
       </c>
+      <c r="B8">
+        <v>207947</v>
+      </c>
+      <c r="C8">
+        <v>1084</v>
+      </c>
+      <c r="D8">
+        <v>51.455111500000697</v>
+      </c>
       <c r="G8">
         <v>1</v>
       </c>
@@ -705,6 +735,15 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
+      </c>
+      <c r="B9">
+        <v>221230</v>
+      </c>
+      <c r="C9">
+        <v>1158</v>
+      </c>
+      <c r="D9">
+        <v>50.072432500001</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -726,6 +765,15 @@
       <c r="A10" s="1">
         <v>5</v>
       </c>
+      <c r="B10">
+        <v>222623</v>
+      </c>
+      <c r="C10">
+        <v>1162</v>
+      </c>
+      <c r="D10">
+        <v>44.838050300000702</v>
+      </c>
       <c r="G10">
         <v>1</v>
       </c>
@@ -746,6 +794,15 @@
       <c r="A11" s="1">
         <v>6</v>
       </c>
+      <c r="B11">
+        <v>167513</v>
+      </c>
+      <c r="C11">
+        <v>873</v>
+      </c>
+      <c r="D11">
+        <v>41.213411700000499</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
@@ -766,6 +823,15 @@
       <c r="A12" s="1">
         <v>7</v>
       </c>
+      <c r="B12">
+        <v>218001</v>
+      </c>
+      <c r="C12">
+        <v>1135</v>
+      </c>
+      <c r="D12">
+        <v>53.512369100001202</v>
+      </c>
       <c r="G12">
         <v>1</v>
       </c>
@@ -785,6 +851,15 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
+      </c>
+      <c r="B13">
+        <v>180548</v>
+      </c>
+      <c r="C13">
+        <v>942</v>
+      </c>
+      <c r="D13">
+        <v>45.9892784000007</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -806,9 +881,15 @@
       <c r="A14" s="4">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14">
+        <v>101653</v>
+      </c>
+      <c r="C14">
+        <v>527</v>
+      </c>
+      <c r="D14">
+        <v>21.7470286</v>
+      </c>
       <c r="G14">
         <v>1</v>
       </c>
@@ -832,6 +913,15 @@
       <c r="A15" s="1">
         <v>10</v>
       </c>
+      <c r="B15">
+        <v>172005</v>
+      </c>
+      <c r="C15">
+        <v>893</v>
+      </c>
+      <c r="D15">
+        <v>44.407744800000501</v>
+      </c>
       <c r="G15">
         <v>1</v>
       </c>
@@ -1051,7 +1141,21 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
+      <c r="A26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>185063.5</v>
+      </c>
+      <c r="C26">
+        <v>964</v>
+      </c>
+      <c r="D26">
+        <v>44.536797160000702</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="M26" s="7"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -1066,7 +1170,15 @@
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29">
+        <v>232998</v>
+      </c>
+      <c r="C29">
+        <v>1227</v>
+      </c>
+      <c r="D29">
+        <v>43.757262200001001</v>
+      </c>
       <c r="G29">
         <v>1</v>
       </c>
@@ -1087,7 +1199,15 @@
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30">
+        <v>121304</v>
+      </c>
+      <c r="C30">
+        <v>639</v>
+      </c>
+      <c r="D30">
+        <v>21.450398100000001</v>
+      </c>
       <c r="G30">
         <v>1</v>
       </c>
@@ -1108,7 +1228,15 @@
       <c r="A31">
         <v>3</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31">
+        <v>205892</v>
+      </c>
+      <c r="C31">
+        <v>1084</v>
+      </c>
+      <c r="D31">
+        <v>37.975007200000597</v>
+      </c>
       <c r="G31">
         <v>1</v>
       </c>
@@ -1129,7 +1257,15 @@
       <c r="A32">
         <v>4</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32">
+        <v>219861</v>
+      </c>
+      <c r="C32">
+        <v>1158</v>
+      </c>
+      <c r="D32">
+        <v>37.982350200000603</v>
+      </c>
       <c r="G32">
         <v>1</v>
       </c>
@@ -1150,7 +1286,15 @@
       <c r="A33">
         <v>5</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33">
+        <v>220635</v>
+      </c>
+      <c r="C33">
+        <v>1162</v>
+      </c>
+      <c r="D33">
+        <v>40.836220100000702</v>
+      </c>
       <c r="G33">
         <v>1</v>
       </c>
@@ -1171,7 +1315,15 @@
       <c r="A34">
         <v>6</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34">
+        <v>165788</v>
+      </c>
+      <c r="C34">
+        <v>873</v>
+      </c>
+      <c r="D34">
+        <v>29.720212900000298</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
@@ -1192,7 +1344,15 @@
       <c r="A35">
         <v>7</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35">
+        <v>215605</v>
+      </c>
+      <c r="C35">
+        <v>1135</v>
+      </c>
+      <c r="D35">
+        <v>40.0553936000005</v>
+      </c>
       <c r="G35">
         <v>1</v>
       </c>
@@ -1213,7 +1373,15 @@
       <c r="A36">
         <v>8</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36">
+        <v>178866</v>
+      </c>
+      <c r="C36">
+        <v>942</v>
+      </c>
+      <c r="D36">
+        <v>32.112510200000301</v>
+      </c>
       <c r="G36">
         <v>1</v>
       </c>
@@ -1234,7 +1402,15 @@
       <c r="A37">
         <v>9</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37">
+        <v>100006</v>
+      </c>
+      <c r="C37">
+        <v>527</v>
+      </c>
+      <c r="D37">
+        <v>17.648483099999901</v>
+      </c>
       <c r="G37">
         <v>1</v>
       </c>
@@ -1255,7 +1431,15 @@
       <c r="A38">
         <v>10</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38">
+        <v>169447</v>
+      </c>
+      <c r="C38">
+        <v>893</v>
+      </c>
+      <c r="D38">
+        <v>31.450612600000301</v>
+      </c>
       <c r="G38">
         <v>1</v>
       </c>
@@ -1482,6 +1666,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49">
+        <v>183040.2</v>
+      </c>
+      <c r="C49">
+        <v>964</v>
+      </c>
+      <c r="D49">
+        <v>33.2988450200004</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>16</v>
@@ -1546,7 +1747,7 @@
       <c r="B56" s="1"/>
       <c r="D56" s="1"/>
       <c r="G56">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>8</v>
@@ -1568,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>8</v>
@@ -1588,7 +1789,7 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>8</v>
@@ -1608,7 +1809,7 @@
         <v>3</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>8</v>
@@ -1628,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>8</v>
@@ -1648,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>8</v>
@@ -1668,7 +1869,7 @@
         <v>6</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>8</v>
@@ -1688,7 +1889,7 @@
         <v>7</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>8</v>
@@ -1708,7 +1909,7 @@
         <v>8</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>8</v>
@@ -1731,7 +1932,7 @@
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="G65">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>8</v>
@@ -1754,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>8</v>
@@ -1774,7 +1975,7 @@
         <v>11</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>8</v>
@@ -1794,7 +1995,7 @@
         <v>12</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>8</v>
@@ -1815,7 +2016,7 @@
       </c>
       <c r="B69" s="1"/>
       <c r="G69">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>8</v>
@@ -1836,7 +2037,7 @@
         <v>14</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>8</v>
@@ -1856,7 +2057,7 @@
         <v>15</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>8</v>
@@ -1876,7 +2077,7 @@
         <v>16</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>8</v>
@@ -1896,7 +2097,7 @@
         <v>17</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>8</v>
@@ -1916,7 +2117,7 @@
         <v>18</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>8</v>
@@ -1936,7 +2137,7 @@
         <v>19</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>8</v>
@@ -1956,7 +2157,7 @@
         <v>20</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>8</v>
@@ -1972,7 +2173,13 @@
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B77" s="7"/>
+      <c r="L77" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="M77" s="7"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -1989,7 +2196,7 @@
       </c>
       <c r="B80" s="1"/>
       <c r="G80">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>4</v>
@@ -2010,7 +2217,7 @@
       </c>
       <c r="B81" s="1"/>
       <c r="G81">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>4</v>
@@ -2031,7 +2238,7 @@
       </c>
       <c r="B82" s="1"/>
       <c r="G82">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>4</v>
@@ -2052,7 +2259,7 @@
       </c>
       <c r="B83" s="1"/>
       <c r="G83">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>4</v>
@@ -2073,7 +2280,7 @@
       </c>
       <c r="B84" s="1"/>
       <c r="G84">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>4</v>
@@ -2094,7 +2301,7 @@
       </c>
       <c r="B85" s="1"/>
       <c r="G85">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>4</v>
@@ -2115,7 +2322,7 @@
       </c>
       <c r="B86" s="1"/>
       <c r="G86">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>4</v>
@@ -2136,7 +2343,7 @@
       </c>
       <c r="B87" s="1"/>
       <c r="G87">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>4</v>
@@ -2157,7 +2364,7 @@
       </c>
       <c r="B88" s="1"/>
       <c r="G88">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>4</v>
@@ -2178,7 +2385,7 @@
       </c>
       <c r="B89" s="1"/>
       <c r="G89">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>4</v>
@@ -2199,7 +2406,7 @@
       </c>
       <c r="B90" s="1"/>
       <c r="G90">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>4</v>
@@ -2220,7 +2427,7 @@
       </c>
       <c r="B91" s="1"/>
       <c r="G91">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>4</v>
@@ -2241,7 +2448,7 @@
       </c>
       <c r="B92" s="1"/>
       <c r="G92">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>4</v>
@@ -2262,7 +2469,7 @@
       </c>
       <c r="B93" s="1"/>
       <c r="G93">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>4</v>
@@ -2283,7 +2490,7 @@
       </c>
       <c r="B94" s="1"/>
       <c r="G94">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>4</v>
@@ -2304,7 +2511,7 @@
       </c>
       <c r="B95" s="1"/>
       <c r="G95">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>4</v>
@@ -2325,7 +2532,7 @@
       </c>
       <c r="B96" s="1"/>
       <c r="G96">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>4</v>
@@ -2346,7 +2553,7 @@
       </c>
       <c r="B97" s="1"/>
       <c r="G97">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>4</v>
@@ -2367,7 +2574,7 @@
       </c>
       <c r="B98" s="1"/>
       <c r="G98">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>4</v>
@@ -2388,7 +2595,7 @@
       </c>
       <c r="B99" s="1"/>
       <c r="G99">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>4</v>
@@ -2401,6 +2608,46 @@
       </c>
       <c r="R99" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L100" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>43.757262200001001</v>
+      </c>
+      <c r="C109">
+        <v>21.450398100000001</v>
+      </c>
+      <c r="D109">
+        <v>37.975007200000597</v>
+      </c>
+      <c r="E109">
+        <v>37.982350200000603</v>
+      </c>
+      <c r="F109">
+        <v>40.836220100000702</v>
+      </c>
+      <c r="G109">
+        <v>29.720212900000298</v>
+      </c>
+      <c r="H109">
+        <v>40.0553936000005</v>
+      </c>
+      <c r="I109">
+        <v>32.112510200000301</v>
+      </c>
+      <c r="J109">
+        <v>17.648483099999901</v>
+      </c>
+      <c r="K109">
+        <v>31.450612600000301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed results of RL Test 1
</commit_message>
<xml_diff>
--- a/pyFiles/RL/Results/New Results/ResultsDQNdecayEpsilon.xlsx
+++ b/pyFiles/RL/Results/New Results/ResultsDQNdecayEpsilon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozho1\Desktop\Thesis Code\ThesisWorkCybercom\pyFiles\RL\Results\New Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A39111-EF99-4F60-82D5-3FABE2D288F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB4197A-08B9-409A-A2BB-0DE1514795F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1BC5E51A-5632-4252-887C-9C128D35FB87}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="21">
   <si>
     <t>Controller</t>
   </si>
@@ -104,13 +104,16 @@
     <t>Until all node dies</t>
   </si>
   <si>
-    <t>Mean</t>
-  </si>
-  <si>
     <t>Mean 1J</t>
   </si>
   <si>
     <t>Mean 0.05J</t>
+  </si>
+  <si>
+    <t>Mean 0.05</t>
+  </si>
+  <si>
+    <t>Pac. per Joule</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -226,6 +229,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2693EA75-5C63-4FDE-887F-C7326CFE699C}">
-  <dimension ref="A1:R100"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,21 +565,26 @@
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="34.7109375" customWidth="1"/>
     <col min="14" max="15" width="18" customWidth="1"/>
-    <col min="17" max="17" width="19" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L2" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -589,7 +598,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,6 +611,9 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
@@ -620,14 +632,17 @@
       <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="P4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -644,14 +659,14 @@
       </c>
       <c r="M5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -664,6 +679,10 @@
       <c r="D6">
         <v>48.552244900001099</v>
       </c>
+      <c r="E6">
+        <f>B6/D6</f>
+        <v>4863.3590575745893</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
@@ -673,14 +692,14 @@
       <c r="L6" s="1">
         <v>1</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -693,6 +712,10 @@
       <c r="D7">
         <v>43.580299800000397</v>
       </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E51" si="0">B7/D7</f>
+        <v>2822.1008245564863</v>
+      </c>
       <c r="G7">
         <v>1</v>
       </c>
@@ -702,14 +725,14 @@
       <c r="L7" s="1">
         <v>2</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -722,6 +745,10 @@
       <c r="D8">
         <v>51.455111500000697</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4041.3283333376353</v>
+      </c>
       <c r="G8">
         <v>1</v>
       </c>
@@ -731,14 +758,14 @@
       <c r="L8" s="1">
         <v>3</v>
       </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -751,6 +778,10 @@
       <c r="D9">
         <v>50.072432500001</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>4418.1995751853192</v>
+      </c>
       <c r="G9">
         <v>1</v>
       </c>
@@ -760,14 +791,14 @@
       <c r="L9" s="1">
         <v>4</v>
       </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -780,6 +811,10 @@
       <c r="D10">
         <v>44.838050300000702</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>4965.0463949811065</v>
+      </c>
       <c r="G10">
         <v>1</v>
       </c>
@@ -789,14 +824,14 @@
       <c r="L10" s="1">
         <v>5</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -809,6 +844,10 @@
       <c r="D11">
         <v>41.213411700000499</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>4064.5264027000699</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
@@ -818,14 +857,14 @@
       <c r="L11" s="1">
         <v>6</v>
       </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -838,6 +877,10 @@
       <c r="D12">
         <v>53.512369100001202</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4073.8431817999085</v>
+      </c>
       <c r="G12">
         <v>1</v>
       </c>
@@ -847,14 +890,14 @@
       <c r="L12" s="1">
         <v>7</v>
       </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -867,6 +910,10 @@
       <c r="D13">
         <v>45.9892784000007</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3925.8715570539862</v>
+      </c>
       <c r="G13">
         <v>1</v>
       </c>
@@ -876,14 +923,14 @@
       <c r="L13" s="1">
         <v>8</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>9</v>
       </c>
@@ -895,6 +942,10 @@
       </c>
       <c r="D14">
         <v>21.7470286</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>4674.3397394529566</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -908,14 +959,14 @@
       <c r="M14" s="4"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -928,6 +979,10 @@
       <c r="D15">
         <v>44.407744800000501</v>
       </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>3873.3108554523592</v>
+      </c>
       <c r="G15">
         <v>1</v>
       </c>
@@ -937,14 +992,14 @@
       <c r="L15" s="1">
         <v>10</v>
       </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -957,6 +1012,10 @@
       <c r="D16">
         <v>2.8225883999999901</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>5189.5628849038176</v>
+      </c>
       <c r="G16">
         <v>0.05</v>
       </c>
@@ -966,14 +1025,14 @@
       <c r="L16" s="1">
         <v>11</v>
       </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0.05</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -986,6 +1045,10 @@
       <c r="D17">
         <v>2.5925128999999898</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>5285.6053290998298</v>
+      </c>
       <c r="G17">
         <v>0.05</v>
       </c>
@@ -995,14 +1058,14 @@
       <c r="L17" s="1">
         <v>12</v>
       </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>0.05</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1015,6 +1078,10 @@
       <c r="D18">
         <v>2.1257920999999902</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4617.5729037661049</v>
+      </c>
       <c r="G18">
         <v>0.05</v>
       </c>
@@ -1025,14 +1092,14 @@
         <v>13</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>0.05</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1045,6 +1112,10 @@
       <c r="D19">
         <v>2.23126489999999</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>5189.88130902792</v>
+      </c>
       <c r="G19">
         <v>0.05</v>
       </c>
@@ -1054,14 +1125,14 @@
       <c r="L19" s="1">
         <v>14</v>
       </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>0.05</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1074,6 +1145,10 @@
       <c r="D20">
         <v>1.93578939999999</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>3599.0485328621162</v>
+      </c>
       <c r="G20">
         <v>0.05</v>
       </c>
@@ -1083,14 +1158,14 @@
       <c r="L20" s="1">
         <v>15</v>
       </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>0.05</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1103,6 +1178,10 @@
       <c r="D21">
         <v>2.3530492999999901</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>5075.1167856959264</v>
+      </c>
       <c r="G21">
         <v>0.05</v>
       </c>
@@ -1112,14 +1191,14 @@
       <c r="L21" s="1">
         <v>16</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>0.05</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1132,6 +1211,10 @@
       <c r="D22">
         <v>2.5155277999999899</v>
       </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>5834.1633115722507</v>
+      </c>
       <c r="G22">
         <v>0.05</v>
       </c>
@@ -1141,14 +1224,14 @@
       <c r="L22" s="1">
         <v>17</v>
       </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>0.05</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>18</v>
       </c>
@@ -1161,6 +1244,10 @@
       <c r="D23">
         <v>1.8578850999999901</v>
       </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>5249.5173140685893</v>
+      </c>
       <c r="G23">
         <v>0.05</v>
       </c>
@@ -1170,14 +1257,14 @@
       <c r="L23" s="1">
         <v>18</v>
       </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>0.05</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -1190,6 +1277,10 @@
       <c r="D24">
         <v>2.1803552000000002</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>4616.6789704723333</v>
+      </c>
       <c r="G24">
         <v>0.05</v>
       </c>
@@ -1199,14 +1290,14 @@
       <c r="L24" s="1">
         <v>19</v>
       </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>0.05</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -1219,6 +1310,10 @@
       <c r="D25">
         <v>2.1269175999999899</v>
       </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>4715.2743481929192</v>
+      </c>
       <c r="G25">
         <v>0.05</v>
       </c>
@@ -1228,16 +1323,16 @@
       <c r="L25" s="1">
         <v>20</v>
       </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>0.05</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26">
         <v>185063.5</v>
@@ -1248,14 +1343,18 @@
       <c r="D26">
         <v>44.536797160000702</v>
       </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>4155.2943139388763</v>
+      </c>
       <c r="L26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27">
         <v>11318</v>
@@ -1266,13 +1365,20 @@
       <c r="D27">
         <v>2.2741682699999899</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>4976.7645381843495</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C28" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>7</v>
       </c>
@@ -1280,7 +1386,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1293,23 +1399,27 @@
       <c r="D30">
         <v>43.757262200001001</v>
       </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>5324.7846936821079</v>
+      </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-      <c r="Q30">
-        <v>1</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1322,23 +1432,27 @@
       <c r="D31">
         <v>21.450398100000001</v>
       </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>5655.0931798324054</v>
+      </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <v>2</v>
       </c>
-      <c r="Q31">
-        <v>1</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1351,23 +1465,27 @@
       <c r="D32">
         <v>37.975007200000597</v>
       </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>5421.7764572272881</v>
+      </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <v>3</v>
       </c>
-      <c r="Q32">
-        <v>1</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1380,23 +1498,27 @@
       <c r="D33">
         <v>37.982350200000603</v>
       </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>5788.5043669571696</v>
+      </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L33">
-        <v>4</v>
-      </c>
-      <c r="Q33">
-        <v>1</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L33" s="1">
+        <v>4</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -1409,23 +1531,27 @@
       <c r="D34">
         <v>40.836220100000702</v>
       </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>5402.924155558565</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1">
         <v>5</v>
       </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -1438,23 +1564,27 @@
       <c r="D35">
         <v>29.720212900000298</v>
       </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>5578.2911299399993</v>
+      </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="1">
         <v>6</v>
       </c>
-      <c r="Q35">
-        <v>1</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>1</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -1467,23 +1597,27 @@
       <c r="D36">
         <v>40.0553936000005</v>
       </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>5382.6708620832851</v>
+      </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1">
         <v>7</v>
       </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -1496,23 +1630,27 @@
       <c r="D37">
         <v>32.112510200000301</v>
       </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>5569.9787679630954</v>
+      </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L37">
-        <v>8</v>
-      </c>
-      <c r="Q37">
-        <v>1</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L37" s="1">
+        <v>8</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1525,23 +1663,30 @@
       <c r="D38">
         <v>17.648483099999901</v>
       </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>5666.5493251372163</v>
+      </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="4">
         <v>9</v>
       </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M38" s="4"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1554,23 +1699,27 @@
       <c r="D39">
         <v>31.450612600000301</v>
       </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>5387.7169947398215</v>
+      </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1">
         <v>10</v>
       </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11</v>
       </c>
@@ -1583,23 +1732,27 @@
       <c r="D40">
         <v>2.8083561999999902</v>
       </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>5171.3525513608465</v>
+      </c>
       <c r="G40">
         <v>0.05</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <v>11</v>
       </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>0.05</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
@@ -1612,23 +1765,27 @@
       <c r="D41">
         <v>2.5415984999999899</v>
       </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>5317.1262101390339</v>
+      </c>
       <c r="G41">
         <v>0.05</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="1">
         <v>12</v>
       </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>0.05</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>13</v>
       </c>
@@ -1641,23 +1798,28 @@
       <c r="D42">
         <v>1.8884569999999901</v>
       </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>5183.0674460684313</v>
+      </c>
       <c r="G42">
         <v>0.05</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="1">
         <v>13</v>
       </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M42" s="1"/>
+      <c r="R42">
+        <v>0.05</v>
+      </c>
+      <c r="S42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>14</v>
       </c>
@@ -1670,23 +1832,27 @@
       <c r="D43">
         <v>2.18580989999999</v>
       </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>5295.5199809462174</v>
+      </c>
       <c r="G43">
         <v>0.05</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
         <v>14</v>
       </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>0.05</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>15</v>
       </c>
@@ -1699,23 +1865,27 @@
       <c r="D44">
         <v>1.2164315000000001</v>
       </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>5696.1694924868352</v>
+      </c>
       <c r="G44">
         <v>0.05</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1">
         <v>15</v>
       </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-      <c r="R44" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>0.05</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>16</v>
       </c>
@@ -1728,23 +1898,27 @@
       <c r="D45">
         <v>2.2793097999999898</v>
       </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>5228.3371045042022</v>
+      </c>
       <c r="G45">
         <v>0.05</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="1">
         <v>16</v>
       </c>
-      <c r="Q45">
-        <v>1</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>0.05</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>17</v>
       </c>
@@ -1757,23 +1931,27 @@
       <c r="D46">
         <v>2.4869780999999902</v>
       </c>
+      <c r="E46">
+        <f t="shared" si="0"/>
+        <v>5867.3616788181844</v>
+      </c>
       <c r="G46">
         <v>0.05</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="1">
         <v>17</v>
       </c>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-      <c r="R46" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>0.05</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18</v>
       </c>
@@ -1786,23 +1964,27 @@
       <c r="D47">
         <v>1.7269473</v>
       </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>5573.418482428503</v>
+      </c>
       <c r="G47">
         <v>0.05</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="1">
         <v>18</v>
       </c>
-      <c r="Q47">
-        <v>1</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>0.05</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>19</v>
       </c>
@@ -1815,23 +1997,27 @@
       <c r="D48">
         <v>1.7953380999999899</v>
       </c>
+      <c r="E48">
+        <f t="shared" si="0"/>
+        <v>5518.7376684091178</v>
+      </c>
       <c r="G48">
         <v>0.05</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="1">
         <v>19</v>
       </c>
-      <c r="Q48">
-        <v>1</v>
-      </c>
-      <c r="R48" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>0.05</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20</v>
       </c>
@@ -1844,25 +2030,29 @@
       <c r="D49">
         <v>1.8068333999999999</v>
       </c>
+      <c r="E49">
+        <f t="shared" si="0"/>
+        <v>5435.4762315108856</v>
+      </c>
       <c r="G49">
         <v>0.05</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="1">
         <v>20</v>
       </c>
-      <c r="Q49">
-        <v>1</v>
-      </c>
-      <c r="R49" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>0.05</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50">
         <v>183040.2</v>
@@ -1873,13 +2063,18 @@
       <c r="D50">
         <v>33.2988450200004</v>
       </c>
+      <c r="E50">
+        <f t="shared" si="0"/>
+        <v>5496.8933574140465</v>
+      </c>
       <c r="L50" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M50" s="7"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51">
         <v>11219.2</v>
@@ -1890,13 +2085,23 @@
       <c r="D51">
         <v>2.0736059799999902</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>5410.478224025981</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L53" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>9</v>
       </c>
@@ -1910,7 +2115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>0</v>
       </c>
@@ -1923,6 +2128,9 @@
       <c r="D55" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E55" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="G55" s="2" t="s">
         <v>2</v>
       </c>
@@ -1941,22 +2149,21 @@
       <c r="O55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q55" s="2" t="s">
+      <c r="P55" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R55" s="2" t="s">
+      <c r="S55" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="G56">
-        <v>0.05</v>
-      </c>
       <c r="H56" s="1" t="s">
         <v>8</v>
       </c>
@@ -1965,28 +2172,27 @@
       </c>
       <c r="M56" s="1"/>
       <c r="O56" s="1"/>
-      <c r="Q56">
-        <v>1</v>
-      </c>
-      <c r="R56" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>1</v>
       </c>
       <c r="B57">
-        <v>26594</v>
+        <v>300209</v>
       </c>
       <c r="C57">
-        <v>217</v>
+        <v>2197</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E57">
+        <f>B57/D57</f>
+        <v>3002.0900000000211</v>
       </c>
       <c r="G57">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>8</v>
@@ -1994,28 +2200,32 @@
       <c r="L57" s="1">
         <v>1</v>
       </c>
-      <c r="Q57">
-        <v>1</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R57">
+        <v>1</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2</v>
       </c>
       <c r="B58">
-        <v>25364</v>
+        <v>386271</v>
       </c>
       <c r="C58">
-        <v>320</v>
+        <v>3196</v>
       </c>
       <c r="D58">
-        <v>5</v>
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E58">
+        <f t="shared" ref="E58:E103" si="1">B58/D58</f>
+        <v>3862.7100000000269</v>
       </c>
       <c r="G58">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>8</v>
@@ -2023,28 +2233,32 @@
       <c r="L58" s="1">
         <v>2</v>
       </c>
-      <c r="Q58">
-        <v>1</v>
-      </c>
-      <c r="R58" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>3</v>
       </c>
       <c r="B59">
-        <v>32731</v>
+        <v>441576</v>
       </c>
       <c r="C59">
-        <v>326</v>
+        <v>3658</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>4415.7600000000311</v>
       </c>
       <c r="G59">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>8</v>
@@ -2052,28 +2266,32 @@
       <c r="L59" s="1">
         <v>3</v>
       </c>
-      <c r="Q59">
-        <v>1</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R59">
+        <v>1</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>4</v>
       </c>
       <c r="B60">
-        <v>26121</v>
+        <v>442810</v>
       </c>
       <c r="C60">
-        <v>315</v>
+        <v>3500</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>4428.1000000000349</v>
       </c>
       <c r="G60">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>8</v>
@@ -2081,28 +2299,32 @@
       <c r="L60" s="1">
         <v>4</v>
       </c>
-      <c r="Q60">
-        <v>1</v>
-      </c>
-      <c r="R60" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R60">
+        <v>1</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>5</v>
       </c>
       <c r="B61">
-        <v>24051</v>
+        <v>409185</v>
       </c>
       <c r="C61">
-        <v>184</v>
+        <v>3374</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>4091.8500000000327</v>
       </c>
       <c r="G61">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>8</v>
@@ -2110,28 +2332,32 @@
       <c r="L61" s="1">
         <v>5</v>
       </c>
-      <c r="Q61">
-        <v>1</v>
-      </c>
-      <c r="R61" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>6</v>
       </c>
       <c r="B62">
-        <v>30721</v>
+        <v>456350</v>
       </c>
       <c r="C62">
-        <v>339</v>
+        <v>3793</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>99.999999999999005</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>4563.5000000000455</v>
       </c>
       <c r="G62">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>8</v>
@@ -2139,28 +2365,32 @@
       <c r="L62" s="1">
         <v>6</v>
       </c>
-      <c r="Q62">
-        <v>1</v>
-      </c>
-      <c r="R62" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>7</v>
       </c>
       <c r="B63">
-        <v>29477</v>
+        <v>428366</v>
       </c>
       <c r="C63">
-        <v>368</v>
+        <v>3130</v>
       </c>
       <c r="D63">
-        <v>5</v>
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>4283.6600000000299</v>
       </c>
       <c r="G63">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>8</v>
@@ -2168,28 +2398,32 @@
       <c r="L63" s="1">
         <v>7</v>
       </c>
-      <c r="Q63">
-        <v>1</v>
-      </c>
-      <c r="R63" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R63">
+        <v>1</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>8</v>
       </c>
       <c r="B64">
-        <v>29642</v>
+        <v>512071</v>
       </c>
       <c r="C64">
-        <v>325</v>
+        <v>4481</v>
       </c>
       <c r="D64">
-        <v>5</v>
+        <v>99.999999999999105</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>5120.7100000000455</v>
       </c>
       <c r="G64">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>8</v>
@@ -2197,28 +2431,32 @@
       <c r="L64" s="1">
         <v>8</v>
       </c>
-      <c r="Q64">
-        <v>1</v>
-      </c>
-      <c r="R64" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>9</v>
       </c>
       <c r="B65">
-        <v>27305</v>
+        <v>341156</v>
       </c>
       <c r="C65">
-        <v>278</v>
-      </c>
-      <c r="D65" s="5">
-        <v>5</v>
+        <v>2531</v>
+      </c>
+      <c r="D65">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>3411.5600000000236</v>
       </c>
       <c r="G65">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>8</v>
@@ -2229,28 +2467,32 @@
       <c r="M65" s="4"/>
       <c r="N65" s="5"/>
       <c r="O65" s="5"/>
-      <c r="Q65">
-        <v>1</v>
-      </c>
-      <c r="R65" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>10</v>
       </c>
       <c r="B66">
-        <v>24195</v>
+        <v>442382</v>
       </c>
       <c r="C66">
-        <v>213</v>
+        <v>3725</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>4423.8200000000352</v>
       </c>
       <c r="G66">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>8</v>
@@ -2258,19 +2500,32 @@
       <c r="L66" s="1">
         <v>10</v>
       </c>
-      <c r="Q66">
-        <v>1</v>
-      </c>
-      <c r="R66" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>11</v>
       </c>
+      <c r="B67">
+        <v>26594</v>
+      </c>
+      <c r="C67">
+        <v>217</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>5318.8</v>
+      </c>
       <c r="G67">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>8</v>
@@ -2278,19 +2533,32 @@
       <c r="L67" s="1">
         <v>11</v>
       </c>
-      <c r="Q67">
-        <v>1</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R67">
+        <v>0.05</v>
+      </c>
+      <c r="S67" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>12</v>
       </c>
+      <c r="B68">
+        <v>25364</v>
+      </c>
+      <c r="C68">
+        <v>320</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>5072.8</v>
+      </c>
       <c r="G68">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>8</v>
@@ -2298,20 +2566,32 @@
       <c r="L68" s="1">
         <v>12</v>
       </c>
-      <c r="Q68">
-        <v>1</v>
-      </c>
-      <c r="R68" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R68">
+        <v>0.05</v>
+      </c>
+      <c r="S68" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>13</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69">
+        <v>32731</v>
+      </c>
+      <c r="C69">
+        <v>326</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>6546.2</v>
+      </c>
       <c r="G69">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>8</v>
@@ -2320,19 +2600,32 @@
         <v>13</v>
       </c>
       <c r="M69" s="1"/>
-      <c r="Q69">
-        <v>1</v>
-      </c>
-      <c r="R69" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <v>0.05</v>
+      </c>
+      <c r="S69" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>14</v>
       </c>
+      <c r="B70">
+        <v>26121</v>
+      </c>
+      <c r="C70">
+        <v>315</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>5224.2</v>
+      </c>
       <c r="G70">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>8</v>
@@ -2340,19 +2633,32 @@
       <c r="L70" s="1">
         <v>14</v>
       </c>
-      <c r="Q70">
-        <v>1</v>
-      </c>
-      <c r="R70" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <v>0.05</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>15</v>
       </c>
+      <c r="B71">
+        <v>24051</v>
+      </c>
+      <c r="C71">
+        <v>184</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>4810.2</v>
+      </c>
       <c r="G71">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>8</v>
@@ -2360,19 +2666,32 @@
       <c r="L71" s="1">
         <v>15</v>
       </c>
-      <c r="Q71">
-        <v>1</v>
-      </c>
-      <c r="R71" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R71">
+        <v>0.05</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>16</v>
       </c>
+      <c r="B72">
+        <v>30721</v>
+      </c>
+      <c r="C72">
+        <v>339</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="1"/>
+        <v>6144.2</v>
+      </c>
       <c r="G72">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>8</v>
@@ -2380,19 +2699,32 @@
       <c r="L72" s="1">
         <v>16</v>
       </c>
-      <c r="Q72">
-        <v>1</v>
-      </c>
-      <c r="R72" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R72">
+        <v>0.05</v>
+      </c>
+      <c r="S72" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>17</v>
       </c>
+      <c r="B73">
+        <v>29477</v>
+      </c>
+      <c r="C73">
+        <v>368</v>
+      </c>
+      <c r="D73">
+        <v>5</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="1"/>
+        <v>5895.4</v>
+      </c>
       <c r="G73">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>8</v>
@@ -2400,19 +2732,32 @@
       <c r="L73" s="1">
         <v>17</v>
       </c>
-      <c r="Q73">
-        <v>1</v>
-      </c>
-      <c r="R73" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R73">
+        <v>0.05</v>
+      </c>
+      <c r="S73" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>18</v>
       </c>
+      <c r="B74">
+        <v>29642</v>
+      </c>
+      <c r="C74">
+        <v>325</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>5928.4</v>
+      </c>
       <c r="G74">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>8</v>
@@ -2420,19 +2765,32 @@
       <c r="L74" s="1">
         <v>18</v>
       </c>
-      <c r="Q74">
-        <v>1</v>
-      </c>
-      <c r="R74" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <v>0.05</v>
+      </c>
+      <c r="S74" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>19</v>
       </c>
+      <c r="B75">
+        <v>27305</v>
+      </c>
+      <c r="C75">
+        <v>278</v>
+      </c>
+      <c r="D75" s="5">
+        <v>5</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="1"/>
+        <v>5461</v>
+      </c>
       <c r="G75">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>8</v>
@@ -2440,19 +2798,32 @@
       <c r="L75" s="1">
         <v>19</v>
       </c>
-      <c r="Q75">
-        <v>1</v>
-      </c>
-      <c r="R75" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R75">
+        <v>0.05</v>
+      </c>
+      <c r="S75" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>20</v>
       </c>
+      <c r="B76">
+        <v>24195</v>
+      </c>
+      <c r="C76">
+        <v>213</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="1"/>
+        <v>4839</v>
+      </c>
       <c r="G76">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>8</v>
@@ -2460,554 +2831,773 @@
       <c r="L76" s="1">
         <v>20</v>
       </c>
-      <c r="Q76">
-        <v>1</v>
-      </c>
-      <c r="R76" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R76">
+        <v>0.05</v>
+      </c>
+      <c r="S76" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B77">
-        <v>27620.1</v>
+        <v>416037.6</v>
       </c>
       <c r="C77">
-        <v>288.5</v>
+        <v>3358.5</v>
       </c>
       <c r="D77">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="1"/>
+        <v>4160.3760000000002</v>
       </c>
       <c r="L77" s="6" t="s">
         <v>17</v>
       </c>
       <c r="M77" s="7"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B78">
+        <v>27620.1</v>
+      </c>
+      <c r="C78">
+        <v>288.5</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="1"/>
+        <v>5524.0199999999995</v>
+      </c>
+      <c r="L78" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L79" s="6" t="s">
+      <c r="L81" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>1</v>
-      </c>
-      <c r="B80">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1</v>
+      </c>
+      <c r="B82">
+        <v>643339</v>
+      </c>
+      <c r="C82">
+        <v>8864</v>
+      </c>
+      <c r="D82">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>6433.3900000000449</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L82" s="1">
+        <v>1</v>
+      </c>
+      <c r="R82">
+        <v>1</v>
+      </c>
+      <c r="S82" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2</v>
+      </c>
+      <c r="B83">
+        <v>638142</v>
+      </c>
+      <c r="C83">
+        <v>8492</v>
+      </c>
+      <c r="D83">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="1"/>
+        <v>6381.4200000000446</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L83" s="1">
+        <v>2</v>
+      </c>
+      <c r="R83">
+        <v>1</v>
+      </c>
+      <c r="S83" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>646173</v>
+      </c>
+      <c r="C84">
+        <v>8386</v>
+      </c>
+      <c r="D84">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="1"/>
+        <v>6461.730000000045</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L84" s="1">
+        <v>3</v>
+      </c>
+      <c r="R84">
+        <v>1</v>
+      </c>
+      <c r="S84" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>4</v>
+      </c>
+      <c r="B85">
+        <v>691856</v>
+      </c>
+      <c r="C85">
+        <v>8556</v>
+      </c>
+      <c r="D85">
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="1"/>
+        <v>6918.560000000055</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L85" s="1">
+        <v>4</v>
+      </c>
+      <c r="R85">
+        <v>1</v>
+      </c>
+      <c r="S85" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>5</v>
+      </c>
+      <c r="B86">
+        <v>666968</v>
+      </c>
+      <c r="C86">
+        <v>8451</v>
+      </c>
+      <c r="D86">
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>6669.680000000053</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="1">
+        <v>5</v>
+      </c>
+      <c r="R86">
+        <v>1</v>
+      </c>
+      <c r="S86" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>6</v>
+      </c>
+      <c r="B87">
+        <v>688459</v>
+      </c>
+      <c r="C87">
+        <v>7903</v>
+      </c>
+      <c r="D87">
+        <v>99.999999999999005</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="1"/>
+        <v>6884.5900000000684</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L87" s="1">
+        <v>6</v>
+      </c>
+      <c r="R87">
+        <v>1</v>
+      </c>
+      <c r="S87" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>7</v>
+      </c>
+      <c r="B88">
+        <v>661052</v>
+      </c>
+      <c r="C88">
+        <v>8471</v>
+      </c>
+      <c r="D88">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="1"/>
+        <v>6610.5200000000459</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L88" s="1">
+        <v>7</v>
+      </c>
+      <c r="R88">
+        <v>1</v>
+      </c>
+      <c r="S88" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>8</v>
+      </c>
+      <c r="B89">
+        <v>629943</v>
+      </c>
+      <c r="C89">
+        <v>7803</v>
+      </c>
+      <c r="D89">
+        <v>99.999999999999105</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="1"/>
+        <v>6299.4300000000567</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L89" s="1">
+        <v>8</v>
+      </c>
+      <c r="R89">
+        <v>1</v>
+      </c>
+      <c r="S89" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>9</v>
+      </c>
+      <c r="B90">
+        <v>618274</v>
+      </c>
+      <c r="C90">
+        <v>8698</v>
+      </c>
+      <c r="D90">
+        <v>99.999999999999304</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="1"/>
+        <v>6182.7400000000434</v>
+      </c>
+      <c r="G90">
+        <v>1</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L90" s="4">
+        <v>9</v>
+      </c>
+      <c r="M90" s="4"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="R90">
+        <v>1</v>
+      </c>
+      <c r="S90" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>10</v>
+      </c>
+      <c r="B91">
+        <v>677060</v>
+      </c>
+      <c r="C91">
+        <v>8118</v>
+      </c>
+      <c r="D91">
+        <v>99.999999999999204</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="1"/>
+        <v>6770.600000000054</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="1">
+        <v>10</v>
+      </c>
+      <c r="R91">
+        <v>1</v>
+      </c>
+      <c r="S91" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>11</v>
+      </c>
+      <c r="B92">
         <v>30669</v>
       </c>
-      <c r="C80">
+      <c r="C92">
         <v>378</v>
       </c>
-      <c r="D80">
+      <c r="D92">
         <v>5</v>
       </c>
-      <c r="G80">
-        <v>0.05</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L80">
-        <v>1</v>
-      </c>
-      <c r="Q80">
-        <v>1</v>
-      </c>
-      <c r="R80" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>2</v>
-      </c>
-      <c r="B81">
+      <c r="E92">
+        <f t="shared" si="1"/>
+        <v>6133.8</v>
+      </c>
+      <c r="G92">
+        <v>0.05</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L92" s="1">
+        <v>11</v>
+      </c>
+      <c r="R92">
+        <v>0.05</v>
+      </c>
+      <c r="S92" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>12</v>
+      </c>
+      <c r="B93">
         <v>33523</v>
       </c>
-      <c r="C81">
+      <c r="C93">
         <v>407</v>
       </c>
-      <c r="D81">
+      <c r="D93">
         <v>5</v>
       </c>
-      <c r="G81">
-        <v>0.05</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L81">
-        <v>2</v>
-      </c>
-      <c r="Q81">
-        <v>1</v>
-      </c>
-      <c r="R81" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>3</v>
-      </c>
-      <c r="B82">
+      <c r="E93">
+        <f t="shared" si="1"/>
+        <v>6704.6</v>
+      </c>
+      <c r="G93">
+        <v>0.05</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L93" s="1">
+        <v>12</v>
+      </c>
+      <c r="R93">
+        <v>0.05</v>
+      </c>
+      <c r="S93" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>13</v>
+      </c>
+      <c r="B94">
         <v>33045</v>
       </c>
-      <c r="C82">
+      <c r="C94">
         <v>442</v>
       </c>
-      <c r="D82">
+      <c r="D94">
         <v>5</v>
       </c>
-      <c r="G82">
-        <v>0.05</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L82">
-        <v>3</v>
-      </c>
-      <c r="Q82">
-        <v>1</v>
-      </c>
-      <c r="R82" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>4</v>
-      </c>
-      <c r="B83">
+      <c r="E94">
+        <f t="shared" si="1"/>
+        <v>6609</v>
+      </c>
+      <c r="G94">
+        <v>0.05</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L94" s="1">
+        <v>13</v>
+      </c>
+      <c r="M94" s="1"/>
+      <c r="R94">
+        <v>0.05</v>
+      </c>
+      <c r="S94" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>14</v>
+      </c>
+      <c r="B95">
         <v>29328</v>
       </c>
-      <c r="C83">
+      <c r="C95">
         <v>387</v>
       </c>
-      <c r="D83">
+      <c r="D95">
         <v>5</v>
       </c>
-      <c r="G83">
-        <v>0.05</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L83">
-        <v>4</v>
-      </c>
-      <c r="Q83">
-        <v>1</v>
-      </c>
-      <c r="R83" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="E95">
+        <f t="shared" si="1"/>
+        <v>5865.6</v>
+      </c>
+      <c r="G95">
+        <v>0.05</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L95" s="1">
+        <v>14</v>
+      </c>
+      <c r="R95">
+        <v>0.05</v>
+      </c>
+      <c r="S95" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>15</v>
+      </c>
+      <c r="B96">
+        <v>32379</v>
+      </c>
+      <c r="C96">
+        <v>442</v>
+      </c>
+      <c r="D96">
         <v>5</v>
       </c>
-      <c r="B84">
-        <v>32379</v>
-      </c>
-      <c r="C84">
-        <v>442</v>
-      </c>
-      <c r="D84">
+      <c r="E96">
+        <f t="shared" si="1"/>
+        <v>6475.8</v>
+      </c>
+      <c r="G96">
+        <v>0.05</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L96" s="1">
+        <v>15</v>
+      </c>
+      <c r="R96">
+        <v>0.05</v>
+      </c>
+      <c r="S96" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <v>33175</v>
+      </c>
+      <c r="C97">
+        <v>427</v>
+      </c>
+      <c r="D97">
         <v>5</v>
       </c>
-      <c r="G84">
-        <v>0.05</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L84">
+      <c r="E97">
+        <f t="shared" si="1"/>
+        <v>6635</v>
+      </c>
+      <c r="G97">
+        <v>0.05</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L97" s="1">
+        <v>16</v>
+      </c>
+      <c r="R97">
+        <v>0.05</v>
+      </c>
+      <c r="S97" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>17</v>
+      </c>
+      <c r="B98">
+        <v>31994</v>
+      </c>
+      <c r="C98">
+        <v>450</v>
+      </c>
+      <c r="D98">
         <v>5</v>
       </c>
-      <c r="Q84">
-        <v>1</v>
-      </c>
-      <c r="R84" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>6</v>
-      </c>
-      <c r="B85">
-        <v>33175</v>
-      </c>
-      <c r="C85">
-        <v>427</v>
-      </c>
-      <c r="D85">
+      <c r="E98">
+        <f t="shared" si="1"/>
+        <v>6398.8</v>
+      </c>
+      <c r="G98">
+        <v>0.05</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L98" s="1">
+        <v>17</v>
+      </c>
+      <c r="R98">
+        <v>0.05</v>
+      </c>
+      <c r="S98" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>18</v>
+      </c>
+      <c r="B99">
+        <v>30034</v>
+      </c>
+      <c r="C99">
+        <v>398</v>
+      </c>
+      <c r="D99">
         <v>5</v>
       </c>
-      <c r="G85">
-        <v>0.05</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L85">
-        <v>6</v>
-      </c>
-      <c r="Q85">
-        <v>1</v>
-      </c>
-      <c r="R85" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>7</v>
-      </c>
-      <c r="B86">
-        <v>31994</v>
-      </c>
-      <c r="C86">
-        <v>450</v>
-      </c>
-      <c r="D86">
-        <v>5</v>
-      </c>
-      <c r="G86">
-        <v>0.05</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L86">
-        <v>7</v>
-      </c>
-      <c r="Q86">
-        <v>1</v>
-      </c>
-      <c r="R86" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>8</v>
-      </c>
-      <c r="B87">
-        <v>30034</v>
-      </c>
-      <c r="C87">
-        <v>398</v>
-      </c>
-      <c r="D87">
-        <v>5</v>
-      </c>
-      <c r="G87">
-        <v>0.05</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L87">
-        <v>8</v>
-      </c>
-      <c r="Q87">
-        <v>1</v>
-      </c>
-      <c r="R87" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>9</v>
-      </c>
-      <c r="B88">
+      <c r="E99">
+        <f t="shared" si="1"/>
+        <v>6006.8</v>
+      </c>
+      <c r="G99">
+        <v>0.05</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L99" s="1">
+        <v>18</v>
+      </c>
+      <c r="R99">
+        <v>0.05</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>19</v>
+      </c>
+      <c r="B100">
         <v>29754</v>
       </c>
-      <c r="C88">
+      <c r="C100">
         <v>313</v>
-      </c>
-      <c r="D88">
-        <v>5</v>
-      </c>
-      <c r="G88">
-        <v>0.05</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L88">
-        <v>9</v>
-      </c>
-      <c r="Q88">
-        <v>1</v>
-      </c>
-      <c r="R88" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>10</v>
-      </c>
-      <c r="B89">
-        <v>29858</v>
-      </c>
-      <c r="C89">
-        <v>410</v>
-      </c>
-      <c r="D89">
-        <v>5</v>
-      </c>
-      <c r="G89">
-        <v>0.05</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L89">
-        <v>10</v>
-      </c>
-      <c r="Q89">
-        <v>1</v>
-      </c>
-      <c r="R89" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>11</v>
-      </c>
-      <c r="B90" s="1"/>
-      <c r="G90">
-        <v>1</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L90">
-        <v>11</v>
-      </c>
-      <c r="Q90">
-        <v>1</v>
-      </c>
-      <c r="R90" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>12</v>
-      </c>
-      <c r="B91" s="1"/>
-      <c r="G91">
-        <v>1</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L91">
-        <v>12</v>
-      </c>
-      <c r="Q91">
-        <v>1</v>
-      </c>
-      <c r="R91" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>13</v>
-      </c>
-      <c r="B92" s="1"/>
-      <c r="G92">
-        <v>1</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L92">
-        <v>13</v>
-      </c>
-      <c r="Q92">
-        <v>1</v>
-      </c>
-      <c r="R92" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>14</v>
-      </c>
-      <c r="B93" s="1"/>
-      <c r="G93">
-        <v>1</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L93">
-        <v>14</v>
-      </c>
-      <c r="Q93">
-        <v>1</v>
-      </c>
-      <c r="R93" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>15</v>
-      </c>
-      <c r="B94" s="1"/>
-      <c r="G94">
-        <v>1</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L94">
-        <v>15</v>
-      </c>
-      <c r="Q94">
-        <v>1</v>
-      </c>
-      <c r="R94" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>16</v>
-      </c>
-      <c r="B95" s="1"/>
-      <c r="G95">
-        <v>1</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L95">
-        <v>16</v>
-      </c>
-      <c r="Q95">
-        <v>1</v>
-      </c>
-      <c r="R95" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>17</v>
-      </c>
-      <c r="B96" s="1"/>
-      <c r="G96">
-        <v>1</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L96">
-        <v>17</v>
-      </c>
-      <c r="Q96">
-        <v>1</v>
-      </c>
-      <c r="R96" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>18</v>
-      </c>
-      <c r="B97" s="1"/>
-      <c r="G97">
-        <v>1</v>
-      </c>
-      <c r="H97" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L97">
-        <v>18</v>
-      </c>
-      <c r="Q97">
-        <v>1</v>
-      </c>
-      <c r="R97" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>19</v>
-      </c>
-      <c r="B98" s="1"/>
-      <c r="G98">
-        <v>1</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L98">
-        <v>19</v>
-      </c>
-      <c r="Q98">
-        <v>1</v>
-      </c>
-      <c r="R98" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>20</v>
-      </c>
-      <c r="G99">
-        <v>1</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L99">
-        <v>20</v>
-      </c>
-      <c r="Q99">
-        <v>1</v>
-      </c>
-      <c r="R99" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B100" s="1">
-        <v>31375.9</v>
-      </c>
-      <c r="C100">
-        <v>405.4</v>
       </c>
       <c r="D100">
         <v>5</v>
       </c>
-      <c r="L100" s="6" t="s">
+      <c r="E100">
+        <f t="shared" si="1"/>
+        <v>5950.8</v>
+      </c>
+      <c r="G100">
+        <v>0.05</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L100" s="1">
+        <v>19</v>
+      </c>
+      <c r="R100">
+        <v>0.05</v>
+      </c>
+      <c r="S100" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>20</v>
+      </c>
+      <c r="B101">
+        <v>29858</v>
+      </c>
+      <c r="C101">
+        <v>410</v>
+      </c>
+      <c r="D101">
+        <v>5</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="1"/>
+        <v>5971.6</v>
+      </c>
+      <c r="G101">
+        <v>0.05</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L101" s="1">
+        <v>20</v>
+      </c>
+      <c r="R101">
+        <v>0.05</v>
+      </c>
+      <c r="S101" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="B102">
+        <v>656126.6</v>
+      </c>
+      <c r="C102">
+        <v>8374.2000000000007</v>
+      </c>
+      <c r="D102">
+        <v>100</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="1"/>
+        <v>6561.2659999999996</v>
+      </c>
+      <c r="L102" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M102" s="7"/>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="1">
+        <v>31375.9</v>
+      </c>
+      <c r="C103">
+        <v>405.4</v>
+      </c>
+      <c r="D103">
+        <v>5</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="1"/>
+        <v>6275.18</v>
+      </c>
+      <c r="L103" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C107" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>